<commit_message>
Incluídos testes do ranking da stn
</commit_message>
<xml_diff>
--- a/tpl/relatorios fiscais v2024.99.00.xlsx
+++ b/tpl/relatorios fiscais v2024.99.00.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\tpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E852DC-8344-410A-8007-607F9B0A5BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109955F2-BCDA-463D-AA08-7C2E5E852ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" firstSheet="9" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" firstSheet="33" activeTab="43" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros" sheetId="23" r:id="rId1"/>
@@ -56,6 +56,7 @@
     <sheet name="RGF A1 Consolidado" sheetId="60" r:id="rId41"/>
     <sheet name="RGF A5 Consolidado" sheetId="61" r:id="rId42"/>
     <sheet name="RGF A6 Consolidado" sheetId="62" r:id="rId43"/>
+    <sheet name="Verificações" sheetId="65" r:id="rId44"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="30">'RGF A1 CISA'!$B$2:$F$42</definedName>
@@ -157,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3178" uniqueCount="1325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3258" uniqueCount="1368">
   <si>
     <t>Parâmetro</t>
   </si>
@@ -4338,6 +4339,135 @@
   </si>
   <si>
     <t>Descrição</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Valor 1</t>
+  </si>
+  <si>
+    <t>Valor 2</t>
+  </si>
+  <si>
+    <t>Diferença</t>
+  </si>
+  <si>
+    <t>Detalhe</t>
+  </si>
+  <si>
+    <t>D3_00002</t>
+  </si>
+  <si>
+    <t>Igualdade da Informação de despesas orçamentárias entre os anexos 1 e 2 do RREO</t>
+  </si>
+  <si>
+    <t>Dotação inicial</t>
+  </si>
+  <si>
+    <t>Empenhado - no bimestre</t>
+  </si>
+  <si>
+    <t>Empenhado - até o bimestre</t>
+  </si>
+  <si>
+    <t>Liquidado - no bimestre</t>
+  </si>
+  <si>
+    <t>Liquidado - até o bimestre</t>
+  </si>
+  <si>
+    <t>RPNP</t>
+  </si>
+  <si>
+    <t>D3_00005</t>
+  </si>
+  <si>
+    <t>Igualdade da Receita Corrente Líquida (RCL) entre o Anexo 03 do RREO e os Anexos 01, 02, 03 e 04 do RGF do poder executivo</t>
+  </si>
+  <si>
+    <t>RREO A3 / RGF A1</t>
+  </si>
+  <si>
+    <t>RREO A3 / RGF A2</t>
+  </si>
+  <si>
+    <t>RREO A3 / RGF A3</t>
+  </si>
+  <si>
+    <t>RREO A3 / RGF A4</t>
+  </si>
+  <si>
+    <t>D3_00006</t>
+  </si>
+  <si>
+    <t>Igualdade da Dívida Consolidada Líquida (DCL) entre o Anexo 06 do RREO e o Anexo 02 do RGF do poder executivo</t>
+  </si>
+  <si>
+    <t>Igualdade dos restos a pagar não processados entre o Anexo 01 do RREO e o Anexo 05 do RGF de todos os poderes/órgãos</t>
+  </si>
+  <si>
+    <t>D3_00008</t>
+  </si>
+  <si>
+    <t>D3_00009</t>
+  </si>
+  <si>
+    <t>Igualdade dos restos a pagar processados e não processados entre o Anexo 07 do RREO e o Anexo 05 do RGF de todos os poderes/órgãos</t>
+  </si>
+  <si>
+    <t>D3_00010</t>
+  </si>
+  <si>
+    <t>Igualdade da Receita Corrente Líquida (RCL) no Anexo 01 do RGF de todos os poderes/órgãos</t>
+  </si>
+  <si>
+    <t>RCL</t>
+  </si>
+  <si>
+    <t>RCL ajustada</t>
+  </si>
+  <si>
+    <t>D3_00014</t>
+  </si>
+  <si>
+    <t>Igualdade das Transferências Obrigatórias da União Relativas às Emendas Individuais nos Anexos 01, 02 e 04 do RGF do poder executivo</t>
+  </si>
+  <si>
+    <t>RREO A3 / RGF A1 Exec</t>
+  </si>
+  <si>
+    <t>RREO A3 / RGF A1 Leg</t>
+  </si>
+  <si>
+    <t>D3_00015</t>
+  </si>
+  <si>
+    <t>Igualdade das Transferências Relativas às Emendas Individuais entre o Anexo 03 do RREO e o Anexo 01 do RGF do poder executivo</t>
+  </si>
+  <si>
+    <t>D3_00016</t>
+  </si>
+  <si>
+    <t>Igualdade das Transferências Relativas às Emendas de bancada entre o Anexo 03 do RREO e o Anexo 01 do RGF do poder executivo</t>
+  </si>
+  <si>
+    <t>D3_00017</t>
+  </si>
+  <si>
+    <t>Igualdade entre os Restos a Pagar (Processados e Não-Processados) Pagos no Exercício do Anexo 6 do RREO com os Restos a Pagar (Processados e Não-Processados) Pagos do Anexo 7 do RREO</t>
+  </si>
+  <si>
+    <t>D3_00027</t>
+  </si>
+  <si>
+    <t>erifica a igualdade entre Dotação atualizada, Despesas empenhadas até o bimestre, Despesas Liquidadas até o bimestre nos Anexos 1 e 6</t>
+  </si>
+  <si>
+    <t>D3_00028</t>
+  </si>
+  <si>
+    <t>Igualdade no total das "Receitas Realizadas Até o Bimestre" - Anexo 1 e Anexo 6.</t>
   </si>
 </sst>
 </file>
@@ -6583,7 +6713,7 @@
   </sheetPr>
   <dimension ref="B2:I90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:I6"/>
     </sheetView>
   </sheetViews>
@@ -8643,7 +8773,7 @@
   </sheetPr>
   <dimension ref="B2:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -9593,7 +9723,7 @@
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C35" s="261"/>
       <c r="D35" s="261"/>
@@ -11881,7 +12011,7 @@
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C22" s="261"/>
       <c r="D22" s="261"/>
@@ -11977,7 +12107,7 @@
   </sheetPr>
   <dimension ref="B2:M217"/>
   <sheetViews>
-    <sheetView topLeftCell="A189" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C13" sqref="C13:M203"/>
     </sheetView>
   </sheetViews>
@@ -18792,7 +18922,7 @@
     <row r="207" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B207" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C207" s="261"/>
       <c r="D207" s="261"/>
@@ -25681,7 +25811,7 @@
     <row r="206" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B206" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C206" s="261"/>
       <c r="D206" s="261"/>
@@ -27083,7 +27213,7 @@
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C47" s="261"/>
       <c r="D47" s="261"/>
@@ -28543,7 +28673,7 @@
     <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C111" s="261"/>
       <c r="D111" s="261"/>
@@ -30534,7 +30664,7 @@
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C130" s="261"/>
       <c r="D130" s="261"/>
@@ -31321,7 +31451,7 @@
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C21" s="249"/>
       <c r="D21" s="249"/>
@@ -32143,7 +32273,7 @@
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C19" s="249"/>
       <c r="D19" s="249"/>
@@ -32272,8 +32402,8 @@
   </sheetPr>
   <dimension ref="B2:I227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C117" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F150" sqref="F150"/>
+    <sheetView topLeftCell="C195" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F225" sqref="F225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35322,7 +35452,7 @@
     <row r="207" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B207" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C207" s="249"/>
       <c r="D207" s="249"/>
@@ -35470,10 +35600,7 @@
       </c>
       <c r="D225" s="46"/>
       <c r="E225" s="46"/>
-      <c r="F225" s="46" t="str">
-        <f>paramNomePrefeito</f>
-        <v>JOÃO EDÉCIO GRAEF</v>
-      </c>
+      <c r="F225" s="46"/>
       <c r="G225" s="46"/>
       <c r="H225" t="str">
         <f>paramNomePrefeito</f>
@@ -35968,7 +36095,7 @@
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C24" s="249"/>
       <c r="D24" s="249"/>
@@ -37696,7 +37823,7 @@
     <row r="89" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="370" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C89" s="370"/>
       <c r="D89" s="370"/>
@@ -38346,7 +38473,7 @@
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C32" s="249"/>
       <c r="D32" s="249"/>
@@ -42022,7 +42149,7 @@
     <row r="144" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B144" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C144" s="261"/>
       <c r="D144" s="261"/>
@@ -42815,7 +42942,7 @@
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="395" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C31" s="395"/>
       <c r="D31" s="395"/>
@@ -43349,7 +43476,7 @@
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C38" s="261"/>
       <c r="D38" s="261"/>
@@ -44689,7 +44816,7 @@
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C100" s="249"/>
       <c r="D100" s="249"/>
@@ -45952,7 +46079,7 @@
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C46" s="249"/>
       <c r="D46" s="249"/>
@@ -58116,7 +58243,7 @@
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C31" s="261"/>
       <c r="D31" s="261"/>
@@ -58646,7 +58773,7 @@
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C31" s="261"/>
       <c r="D31" s="261"/>
@@ -59353,7 +59480,7 @@
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C55" s="249"/>
       <c r="D55" s="249"/>
@@ -59979,7 +60106,7 @@
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C44" s="261"/>
       <c r="D44" s="261"/>
@@ -60553,7 +60680,7 @@
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C54" s="261"/>
       <c r="D54" s="261"/>
@@ -62001,7 +62128,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -62451,7 +62578,7 @@
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C34" s="249"/>
       <c r="D34" s="249"/>
@@ -62904,7 +63031,7 @@
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C37" s="249"/>
       <c r="D37" s="249"/>
@@ -64075,7 +64202,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -65545,7 +65672,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -65955,7 +66082,7 @@
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C21" s="249"/>
       <c r="D21" s="249"/>
@@ -67504,7 +67631,7 @@
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C41" s="249"/>
       <c r="D41" s="249"/>
@@ -69179,7 +69306,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -69657,7 +69784,7 @@
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/05/2024 às 14:32:36</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
       </c>
       <c r="C37" s="249"/>
       <c r="D37" s="249"/>
@@ -69761,6 +69888,649 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB90099D-91AC-4F3E-A3E4-80463817A380}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="113.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D2">
+        <f>'RREO A1 BO Despesa'!C$31</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>'RREO A2'!C$206</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>D2-E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D3">
+        <f>'RREO A1 BO Despesa'!D$31</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>'RREO A2'!D$206</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F4" si="0">D3-E3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D4">
+        <f>'RREO A1 BO Despesa'!E$31</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>'RREO A2'!E$206</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D5">
+        <f>'RREO A1 BO Despesa'!F$31</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>'RREO A2'!F$206</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5" si="1">D5-E5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="D6">
+        <f>'RREO A1 BO Despesa'!H$31</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>'RREO A2'!I$206</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6" si="2">D6-E6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D7">
+        <f>'RREO A1 BO Despesa'!I$31</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>'RREO A2'!J$206</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7" si="3">D7-E7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D8">
+        <f>'RREO A1 BO Despesa'!L$31</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>'RREO A2'!M$206</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F15" si="4">D8-E8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1340</v>
+      </c>
+      <c r="D9">
+        <f>'RREO A3'!$O$40</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>'RGF A1 Exec'!K36</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D10">
+        <f>'RREO A3'!$O$40</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>IF(paramBimestre=3,'RGF A2'!D38,'RGF A2'!E38)</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1342</v>
+      </c>
+      <c r="D11">
+        <f>'RREO A3'!$O$40</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>IF(paramBimestre=3,'RGF A3'!D23,'RGF A3'!E23)</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D12">
+        <f>'RREO A3'!$O$40</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>'RGF A4'!C34</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D13">
+        <f>'RREO A6'!F108</f>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>IF(paramBimestre=3,'RGF A2'!D37,'RGF A2'!E37)</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D14">
+        <f>'RREO A1 BO Despesa'!L31</f>
+        <v>0</v>
+      </c>
+      <c r="E14" t="e">
+        <f>'RGF A5 Exec 2 Sem'!J42</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F14" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D15">
+        <f>'RREO A7'!N20</f>
+        <v>0</v>
+      </c>
+      <c r="E15" t="e">
+        <f>'RGF A5 Exec 2 Sem'!E42+'RGF A5 Exec 2 Sem'!I42</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F15" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D16">
+        <f>'RGF A1 Exec'!K36</f>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f>'RGF A1 Leg'!K33</f>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f>D16-E16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D17">
+        <f>'RGF A1 Exec'!K41</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>'RGF A1 Leg'!K38</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>D17-E17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D18">
+        <f>'RREO A3'!$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>'RGF A1 Exec'!K37</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ref="F18:F28" si="5">D18-E18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D19">
+        <f>'RREO A3'!$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f>'RGF A1 Leg'!K34</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ref="F19" si="6">D19-E19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D20">
+        <f>'RREO A3'!$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>IF(paramBimestre=3,'RGF A2'!D39,'RGF A2'!E39)</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D21">
+        <f>'RREO A3'!$O$41</f>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f>'RGF A4'!C35</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D22">
+        <f>D18</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>E18</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D23">
+        <f>'RREO A3'!$O$43</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>'RGF A1 Exec'!K38</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D24">
+        <f>'RREO A6'!I67+'RREO A6'!I68+'RREO A6'!I79+'RREO A6'!I80+'RREO A6'!G67+'RREO A6'!G68+'RREO A6'!G79+'RREO A6'!G80</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f>'RREO A7'!E20+'RREO A7'!K20</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D25">
+        <f>'RREO A1 BO Despesa'!D31</f>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f>'RREO A6'!C67+'RREO A6'!C68+'RREO A6'!C79+'RREO A6'!C80</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D26">
+        <f>'RREO A1 BO Despesa'!F31</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f>'RREO A6'!D67+'RREO A6'!D68+'RREO A6'!D79+'RREO A6'!D80</f>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D27">
+        <f>'RREO A1 BO Despesa'!I31</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>'RREO A6'!E67+'RREO A6'!E68+'RREO A6'!E79+'RREO A6'!E80</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D28">
+        <f>'RREO A1 BO Receita'!G84</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f>'RREO A6'!I36+'RREO A6'!I37+'RREO A6'!I52+'RREO A6'!I53</f>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix: corrigido falhas em fórmulas no template dos relatórios fiscais
</commit_message>
<xml_diff>
--- a/tpl/relatorios fiscais v2024.99.00.xlsx
+++ b/tpl/relatorios fiscais v2024.99.00.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\tpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109955F2-BCDA-463D-AA08-7C2E5E852ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1837B66D-92C7-405D-9747-2C399D037B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" firstSheet="33" activeTab="43" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" firstSheet="28" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros" sheetId="23" r:id="rId1"/>
@@ -9723,7 +9723,7 @@
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C35" s="261"/>
       <c r="D35" s="261"/>
@@ -12011,7 +12011,7 @@
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C22" s="261"/>
       <c r="D22" s="261"/>
@@ -18922,7 +18922,7 @@
     <row r="207" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B207" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C207" s="261"/>
       <c r="D207" s="261"/>
@@ -25811,7 +25811,7 @@
     <row r="206" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B206" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C206" s="261"/>
       <c r="D206" s="261"/>
@@ -27213,7 +27213,7 @@
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C47" s="261"/>
       <c r="D47" s="261"/>
@@ -28673,7 +28673,7 @@
     <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C111" s="261"/>
       <c r="D111" s="261"/>
@@ -30664,7 +30664,7 @@
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C130" s="261"/>
       <c r="D130" s="261"/>
@@ -31451,7 +31451,7 @@
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C21" s="249"/>
       <c r="D21" s="249"/>
@@ -32273,7 +32273,7 @@
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C19" s="249"/>
       <c r="D19" s="249"/>
@@ -35452,7 +35452,7 @@
     <row r="207" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B207" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C207" s="249"/>
       <c r="D207" s="249"/>
@@ -36095,7 +36095,7 @@
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C24" s="249"/>
       <c r="D24" s="249"/>
@@ -37823,7 +37823,7 @@
     <row r="89" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="370" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C89" s="370"/>
       <c r="D89" s="370"/>
@@ -38473,7 +38473,7 @@
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C32" s="249"/>
       <c r="D32" s="249"/>
@@ -42149,7 +42149,7 @@
     <row r="144" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B144" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C144" s="261"/>
       <c r="D144" s="261"/>
@@ -42942,7 +42942,7 @@
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="395" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C31" s="395"/>
       <c r="D31" s="395"/>
@@ -43476,7 +43476,7 @@
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C38" s="261"/>
       <c r="D38" s="261"/>
@@ -44816,7 +44816,7 @@
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C100" s="249"/>
       <c r="D100" s="249"/>
@@ -44956,7 +44956,7 @@
   <dimension ref="B2:P57"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42:N42"/>
+      <selection activeCell="B46" sqref="B46:P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46015,7 +46015,7 @@
       <c r="I43" s="423"/>
       <c r="J43" s="423"/>
       <c r="K43" s="292">
-        <f>$K$41*O43</f>
+        <f>ROUND($K$41*O43,2)</f>
         <v>0</v>
       </c>
       <c r="L43" s="292"/>
@@ -46039,7 +46039,7 @@
       <c r="I44" s="233"/>
       <c r="J44" s="233"/>
       <c r="K44" s="294">
-        <f>$K$41*O44</f>
+        <f>ROUND($K$41*O44,2)</f>
         <v>0</v>
       </c>
       <c r="L44" s="294"/>
@@ -46064,7 +46064,7 @@
       <c r="I45" s="425"/>
       <c r="J45" s="425"/>
       <c r="K45" s="306">
-        <f>$K$41*O45</f>
+        <f>ROUND($K$41*O45,2)</f>
         <v>0</v>
       </c>
       <c r="L45" s="306"/>
@@ -46079,7 +46079,7 @@
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C46" s="249"/>
       <c r="D46" s="249"/>
@@ -58243,7 +58243,7 @@
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C31" s="261"/>
       <c r="D31" s="261"/>
@@ -58773,7 +58773,7 @@
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C31" s="261"/>
       <c r="D31" s="261"/>
@@ -59480,7 +59480,7 @@
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C55" s="249"/>
       <c r="D55" s="249"/>
@@ -60106,7 +60106,7 @@
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C44" s="261"/>
       <c r="D44" s="261"/>
@@ -60680,7 +60680,7 @@
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C54" s="261"/>
       <c r="D54" s="261"/>
@@ -62128,7 +62128,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -62578,7 +62578,7 @@
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C34" s="249"/>
       <c r="D34" s="249"/>
@@ -63031,7 +63031,7 @@
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C37" s="249"/>
       <c r="D37" s="249"/>
@@ -63146,8 +63146,8 @@
   </sheetPr>
   <dimension ref="B2:P54"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64091,7 +64091,7 @@
       <c r="I38" s="421"/>
       <c r="J38" s="421"/>
       <c r="K38" s="405">
-        <f>K33-K34-K35</f>
+        <f>K33-K34-K35-K36-K37</f>
         <v>0</v>
       </c>
       <c r="L38" s="405"/>
@@ -64138,7 +64138,7 @@
       <c r="I40" s="423"/>
       <c r="J40" s="423"/>
       <c r="K40" s="292">
-        <f>$K$38*O40</f>
+        <f>ROUND($K$38*O40,2)</f>
         <v>0</v>
       </c>
       <c r="L40" s="292"/>
@@ -64162,7 +64162,7 @@
       <c r="I41" s="233"/>
       <c r="J41" s="233"/>
       <c r="K41" s="294">
-        <f>$K$38*O41</f>
+        <f>ROUND($K$38*O41,2)</f>
         <v>0</v>
       </c>
       <c r="L41" s="294"/>
@@ -64187,7 +64187,7 @@
       <c r="I42" s="425"/>
       <c r="J42" s="425"/>
       <c r="K42" s="306">
-        <f>$K$38*O42</f>
+        <f>ROUND($K$38*O42,2)</f>
         <v>0</v>
       </c>
       <c r="L42" s="306"/>
@@ -64202,7 +64202,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -65672,7 +65672,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -66082,7 +66082,7 @@
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C21" s="249"/>
       <c r="D21" s="249"/>
@@ -66195,7 +66195,9 @@
   </sheetPr>
   <dimension ref="B2:P52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:J36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -67631,7 +67633,7 @@
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C41" s="249"/>
       <c r="D41" s="249"/>
@@ -69306,7 +69308,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -69784,7 +69786,7 @@
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 19/06/2024 às 11:38:28</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 08/07/2024 às 16:36:25</v>
       </c>
       <c r="C37" s="249"/>
       <c r="D37" s="249"/>
@@ -69895,7 +69897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB90099D-91AC-4F3E-A3E4-80463817A380}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: Ajustes em fórmulas do anexo 8 do RREO.
Linhas 11 e 18.
</commit_message>
<xml_diff>
--- a/tpl/relatorios fiscais v2024.99.00.xlsx
+++ b/tpl/relatorios fiscais v2024.99.00.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\tpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A30244-F326-4D74-95F9-7C70908F5A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6725F67C-778F-492E-A334-F2DC53B73EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" firstSheet="14" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros" sheetId="23" r:id="rId1"/>
@@ -4548,6 +4548,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -6071,7 +6072,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="170" formatCode="&quot;&quot;"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -6158,7 +6162,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC2282F1-3F02-481A-9E13-D2318F264292}" name="tblOutrosAjustesDC" displayName="tblOutrosAjustesDC" ref="A1:B20" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC2282F1-3F02-481A-9E13-D2318F264292}" name="tblOutrosAjustesDC" displayName="tblOutrosAjustesDC" ref="A1:B20" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:B20" xr:uid="{AC2282F1-3F02-481A-9E13-D2318F264292}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F4F29D4E-AAEB-4636-BE31-0DE9AA95CFF4}" name="Descrição"/>
@@ -9725,7 +9729,7 @@
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C35" s="261"/>
       <c r="D35" s="261"/>
@@ -12013,7 +12017,7 @@
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C22" s="261"/>
       <c r="D22" s="261"/>
@@ -18924,7 +18928,7 @@
     <row r="207" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B207" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C207" s="261"/>
       <c r="D207" s="261"/>
@@ -19048,7 +19052,7 @@
   </sheetPr>
   <dimension ref="B2:M216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+    <sheetView topLeftCell="A170" workbookViewId="0">
       <selection activeCell="G204" sqref="G204"/>
     </sheetView>
   </sheetViews>
@@ -25813,7 +25817,7 @@
     <row r="206" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B206" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C206" s="261"/>
       <c r="D206" s="261"/>
@@ -27215,7 +27219,7 @@
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C47" s="261"/>
       <c r="D47" s="261"/>
@@ -28675,7 +28679,7 @@
     <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C111" s="261"/>
       <c r="D111" s="261"/>
@@ -30666,7 +30670,7 @@
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C130" s="261"/>
       <c r="D130" s="261"/>
@@ -31453,7 +31457,7 @@
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C21" s="249"/>
       <c r="D21" s="249"/>
@@ -32275,7 +32279,7 @@
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C19" s="249"/>
       <c r="D19" s="249"/>
@@ -32404,8 +32408,8 @@
   </sheetPr>
   <dimension ref="B2:I227"/>
   <sheetViews>
-    <sheetView topLeftCell="C195" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F225" sqref="F225"/>
+    <sheetView tabSelected="1" topLeftCell="C74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107:H107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33582,7 +33586,7 @@
         <v>0</v>
       </c>
       <c r="H91" s="72">
-        <f>IF(C91&gt;H38,C91-H38,0)</f>
+        <f>IF(MONTH(paramDataBase)=12,IF(C91&gt;H38,C91-H38,0),IF(D91&gt;H38,D91-H38,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -33602,7 +33606,7 @@
         <v>0</v>
       </c>
       <c r="H92" s="32">
-        <f>IF(C92&gt;H39,C92-H39,0)</f>
+        <f>IF(MONTH(paramDataBase)=12,IF(C92&gt;H39,C92-H39,0),IF(D92&gt;H39,D92-H39,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -33622,7 +33626,7 @@
         <v>0</v>
       </c>
       <c r="H93" s="32">
-        <f>IF(C93&gt;H43,C93-H43,0)</f>
+        <f>IF(MONTH(paramDataBase)=12,IF(C93&gt;H43,C93-H43,0),IF(D93&gt;H43,D93-H43,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -33642,7 +33646,7 @@
         <v>0</v>
       </c>
       <c r="H94" s="32">
-        <f>IF(C94&gt;H47,C94-H47,0)</f>
+        <f>IF(MONTH(paramDataBase)=12,IF(C94&gt;H47,C94-H47,0),IF(D94&gt;H47,D94-H47,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -33662,7 +33666,7 @@
         <v>0</v>
       </c>
       <c r="H95" s="32">
-        <f>IF(C95&gt;H51,C95-H51,0)</f>
+        <f>IF(MONTH(paramDataBase)=12,IF(C95&gt;H51,C95-H51,0),IF(D95&gt;H51,D95-H51,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -35454,7 +35458,7 @@
     <row r="207" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B207" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C207" s="249"/>
       <c r="D207" s="249"/>
@@ -35811,6 +35815,11 @@
     <mergeCell ref="B214:H214"/>
     <mergeCell ref="B215:H215"/>
   </mergeCells>
+  <conditionalFormatting sqref="E107:H107">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>E107&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="36" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
@@ -36097,7 +36106,7 @@
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C24" s="249"/>
       <c r="D24" s="249"/>
@@ -37825,7 +37834,7 @@
     <row r="89" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="370" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C89" s="370"/>
       <c r="D89" s="370"/>
@@ -38475,7 +38484,7 @@
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C32" s="249"/>
       <c r="D32" s="249"/>
@@ -42151,7 +42160,7 @@
     <row r="144" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B144" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C144" s="261"/>
       <c r="D144" s="261"/>
@@ -42944,7 +42953,7 @@
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C31" s="261"/>
       <c r="D31" s="261"/>
@@ -43478,7 +43487,7 @@
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C38" s="261"/>
       <c r="D38" s="261"/>
@@ -44532,7 +44541,7 @@
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C78" s="249"/>
       <c r="D78" s="249"/>
@@ -45895,7 +45904,7 @@
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C100" s="249"/>
       <c r="D100" s="249"/>
@@ -58730,7 +58739,7 @@
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C46" s="249"/>
       <c r="D46" s="249"/>
@@ -59323,7 +59332,7 @@
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C31" s="261"/>
       <c r="D31" s="261"/>
@@ -59853,7 +59862,7 @@
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C31" s="261"/>
       <c r="D31" s="261"/>
@@ -60560,7 +60569,7 @@
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C55" s="249"/>
       <c r="D55" s="249"/>
@@ -61186,7 +61195,7 @@
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C44" s="261"/>
       <c r="D44" s="261"/>
@@ -61760,7 +61769,7 @@
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="261" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C54" s="261"/>
       <c r="D54" s="261"/>
@@ -63208,7 +63217,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -63658,7 +63667,7 @@
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C34" s="249"/>
       <c r="D34" s="249"/>
@@ -64111,7 +64120,7 @@
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C37" s="249"/>
       <c r="D37" s="249"/>
@@ -65282,7 +65291,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -66843,7 +66852,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -67162,7 +67171,7 @@
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C21" s="249"/>
       <c r="D21" s="249"/>
@@ -68713,7 +68722,7 @@
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C41" s="249"/>
       <c r="D41" s="249"/>
@@ -70388,7 +70397,7 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C43" s="249"/>
       <c r="D43" s="249"/>
@@ -70866,7 +70875,7 @@
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="249" t="str">
         <f ca="1">_xlfn.CONCAT("Fonte: ",paramFonte,". Emissão em ",TEXT(NOW(),"dd/mm/aaaa \à\s hh:mm:ss"))</f>
-        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 10/09/2024 às 16:29:18</v>
+        <v>Fonte: Sistema MS Excel + SIAPC/PAD, Unidade Responsável: Secretaria da Fazenda / Setor de Contabilidade. Emissão em 04/12/2024 às 15:51:34</v>
       </c>
       <c r="C37" s="249"/>
       <c r="D37" s="249"/>

</xml_diff>